<commit_message>
Statistikk for 3. Desember. Fikset årstall i skriptet, sto til 2016.
</commit_message>
<xml_diff>
--- a/X-Helg 2017 Statistikk.xlsx
+++ b/X-Helg 2017 Statistikk.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$8</definedName>
+    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$22</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>Nick</t>
   </si>
@@ -87,7 +87,88 @@
     <t>SisselHultgreen</t>
   </si>
   <si>
-    <t xml:space="preserve">0 besøk logget i Desember! 2 team deltok! </t>
+    <t>johs1988</t>
+  </si>
+  <si>
+    <t>[#3]* [#2]*  (4)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#3]  (3)</t>
+  </si>
+  <si>
+    <t>siljejandersen</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>minni09</t>
+  </si>
+  <si>
+    <t>[#2]  (3)</t>
+  </si>
+  <si>
+    <t>[#1] [#3]  (2)</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>TeamLadybug&lt;3&lt;3</t>
+  </si>
+  <si>
+    <t>[#1]  (1)</t>
+  </si>
+  <si>
+    <t>[#2]  (1)</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>O-K Haukland</t>
+  </si>
+  <si>
+    <t>GunnarKolskog</t>
+  </si>
+  <si>
+    <t>[#3]  (3)</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Kransa</t>
+  </si>
+  <si>
+    <t>[#1] [#2]  (2)</t>
+  </si>
+  <si>
+    <t>TeamCOR</t>
+  </si>
+  <si>
+    <t>cara2006</t>
+  </si>
+  <si>
+    <t>silyam</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Onyx Black</t>
+  </si>
+  <si>
+    <t>SonjaJ</t>
+  </si>
+  <si>
+    <t>annesto</t>
+  </si>
+  <si>
+    <t>tomnor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 besøk hittil! 16 team deltok! </t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1089,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -1017,11 +1098,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="8" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1031,7 +1112,7 @@
       </c>
       <c r="F1" s="10">
         <f ca="1">NOW()</f>
-        <v>43070.67719722222</v>
+        <v>43073.345530671293</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="39.75" customHeight="1">
@@ -1044,7 +1125,7 @@
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="13" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="G2" s="13"/>
     </row>
@@ -1076,16 +1157,18 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="G4" s="6">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1093,20 +1176,264 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6">
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1"/>
-    <row r="12" spans="1:7" ht="15" customHeight="1"/>
+    <row r="11" spans="1:7">
+      <c r="A11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D2:E2"/>

</xml_diff>

<commit_message>
Statistikk for 5. Des. Nå også med funn på publiseringsdato!
</commit_message>
<xml_diff>
--- a/X-Helg 2017 Statistikk.xlsx
+++ b/X-Helg 2017 Statistikk.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\xhelg-stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\xhelg-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,8 +15,8 @@
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$19</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$22</definedName>
+    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$25</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>Nick</t>
   </si>
@@ -93,9 +93,6 @@
     <t>[#3]* [#2]*  (4)</t>
   </si>
   <si>
-    <t>[#1] [#2] [#3]  (3)</t>
-  </si>
-  <si>
     <t>siljejandersen</t>
   </si>
   <si>
@@ -168,7 +165,46 @@
     <t>tomnor</t>
   </si>
   <si>
-    <t xml:space="preserve">25 besøk hittil! 16 team deltok! </t>
+    <t>[#1] [#2] [#3]  (6)</t>
+  </si>
+  <si>
+    <t>[#1]  (2)</t>
+  </si>
+  <si>
+    <t>[#2] [#3]  (2)</t>
+  </si>
+  <si>
+    <t>[#2]*  (2)</t>
+  </si>
+  <si>
+    <t>[#2]  (2)</t>
+  </si>
+  <si>
+    <t>[#1] [#2]  (4)</t>
+  </si>
+  <si>
+    <t>Team Lynis</t>
+  </si>
+  <si>
+    <t>[#4]  (3)</t>
+  </si>
+  <si>
+    <t>TeamPolhøgda</t>
+  </si>
+  <si>
+    <t>[#5]  (3)</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>dogteam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 besøk hittil! 19 team deltok! </t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1125,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -1112,7 +1148,7 @@
       </c>
       <c r="F1" s="10">
         <f ca="1">NOW()</f>
-        <v>43073.345530671293</v>
+        <v>43074.534704282407</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="39.75" customHeight="1">
@@ -1125,7 +1161,7 @@
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G2" s="13"/>
     </row>
@@ -1157,280 +1193,339 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="E4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="6"/>
       <c r="G4" s="6">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F5" s="6" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="G5" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="G6" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
-        <v>5</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6"/>
       <c r="E7" s="7"/>
       <c r="F7" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G7" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>5</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="E8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="6"/>
       <c r="G8" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G9" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G10" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>30</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G11" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="F12" s="6"/>
       <c r="G12" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="F13" s="6"/>
       <c r="G13" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="F14" s="6"/>
       <c r="G14" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="6"/>
+        <v>49</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="F15" s="6"/>
       <c r="G15" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="6" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
       <c r="F16" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G16" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="E17" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="6"/>
       <c r="G17" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="E18" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="6"/>
       <c r="G18" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
       <c r="F19" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G19" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Statistikk for 6. Desember
</commit_message>
<xml_diff>
--- a/X-Helg 2017 Statistikk.xlsx
+++ b/X-Helg 2017 Statistikk.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\xhelg-stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\xhelg-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,8 +15,8 @@
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$22</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$25</definedName>
+    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$26</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
   <si>
     <t>Nick</t>
   </si>
@@ -171,9 +171,6 @@
     <t>[#1]  (2)</t>
   </si>
   <si>
-    <t>[#2] [#3]  (2)</t>
-  </si>
-  <si>
     <t>[#2]*  (2)</t>
   </si>
   <si>
@@ -204,7 +201,22 @@
     <t>dogteam</t>
   </si>
   <si>
-    <t xml:space="preserve">26 besøk hittil! 19 team deltok! </t>
+    <t>[#5] [#4]  (2)</t>
+  </si>
+  <si>
+    <t>[#2] [#3] [#5] [#4]  (4)</t>
+  </si>
+  <si>
+    <t>Team Takoma</t>
+  </si>
+  <si>
+    <t>[#5]  (2)</t>
+  </si>
+  <si>
+    <t>[#4]  (1)</t>
+  </si>
+  <si>
+    <t>32 besøk fra 20 team</t>
   </si>
 </sst>
 </file>
@@ -1125,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1138,7 +1150,7 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="8" customWidth="1"/>
     <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="8" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1148,7 +1160,7 @@
       </c>
       <c r="F1" s="10">
         <f ca="1">NOW()</f>
-        <v>43074.534704282407</v>
+        <v>43075.542066782407</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="39.75" customHeight="1">
@@ -1161,7 +1173,7 @@
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="13" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G2" s="13"/>
     </row>
@@ -1202,9 +1214,11 @@
       <c r="E4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="G4" s="6">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1222,10 +1236,10 @@
         <v>42</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="G5" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1237,10 +1251,10 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>21</v>
@@ -1278,7 +1292,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6">
@@ -1328,15 +1342,15 @@
         <v>36</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="7" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="G11" s="6">
         <v>3</v>
@@ -1347,14 +1361,16 @@
         <v>36</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="6"/>
+      <c r="E12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G12" s="6">
         <v>3</v>
       </c>
@@ -1364,10 +1380,10 @@
         <v>36</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
@@ -1381,10 +1397,10 @@
         <v>36</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
@@ -1398,10 +1414,10 @@
         <v>36</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
@@ -1412,49 +1428,49 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="6" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="6"/>
+        <v>48</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="F16" s="6"/>
       <c r="G16" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="6"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="G17" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6">
@@ -1463,61 +1479,61 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="E19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="6"/>
       <c r="G19" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="G20" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="E21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="6"/>
       <c r="G21" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1526,6 +1542,23 @@
         <v>25</v>
       </c>
       <c r="G22" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Statistikk oppdatert 8. desember
</commit_message>
<xml_diff>
--- a/X-Helg 2017 Statistikk.xlsx
+++ b/X-Helg 2017 Statistikk.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$23</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$26</definedName>
+    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$28</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
   <si>
     <t>Nick</t>
   </si>
@@ -105,9 +105,6 @@
     <t>[#2]  (3)</t>
   </si>
   <si>
-    <t>[#1] [#3]  (2)</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -171,15 +168,9 @@
     <t>[#1]  (2)</t>
   </si>
   <si>
-    <t>[#2]*  (2)</t>
-  </si>
-  <si>
     <t>[#2]  (2)</t>
   </si>
   <si>
-    <t>[#1] [#2]  (4)</t>
-  </si>
-  <si>
     <t>Team Lynis</t>
   </si>
   <si>
@@ -201,12 +192,6 @@
     <t>dogteam</t>
   </si>
   <si>
-    <t>[#5] [#4]  (2)</t>
-  </si>
-  <si>
-    <t>[#2] [#3] [#5] [#4]  (4)</t>
-  </si>
-  <si>
     <t>Team Takoma</t>
   </si>
   <si>
@@ -216,7 +201,61 @@
     <t>[#4]  (1)</t>
   </si>
   <si>
-    <t>32 besøk fra 20 team</t>
+    <t>[#2]* [#5] [#4]  (8)</t>
+  </si>
+  <si>
+    <t>[#2] [#5] [#8]  (6)</t>
+  </si>
+  <si>
+    <t>[#1] [#3] [#4] [#6]  (4)</t>
+  </si>
+  <si>
+    <t>[#5] [#4] [#6]  (3)</t>
+  </si>
+  <si>
+    <t>[#2] [#3] [#5] [#4] [#6]  (5)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#6]  (6)</t>
+  </si>
+  <si>
+    <t>[#3]  (1)</t>
+  </si>
+  <si>
+    <t>[#6]  (3)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#6] [#3]  (4)</t>
+  </si>
+  <si>
+    <t>[#1] [#3] [#6]  (3)</t>
+  </si>
+  <si>
+    <t>[#8]  (2)</t>
+  </si>
+  <si>
+    <t>[#2] [#6] [#3]  (3)</t>
+  </si>
+  <si>
+    <t>anila65</t>
+  </si>
+  <si>
+    <t>[#6] [#1] [#2] [#3]  (4)</t>
+  </si>
+  <si>
+    <t>TeamAlmli</t>
+  </si>
+  <si>
+    <t>[#8]  (3)</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>50 besøk fra 22 team!</t>
   </si>
 </sst>
 </file>
@@ -1137,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1148,9 +1187,9 @@
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="8" customWidth="1"/>
     <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="8" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1160,7 +1199,7 @@
       </c>
       <c r="F1" s="10">
         <f ca="1">NOW()</f>
-        <v>43075.542066782407</v>
+        <v>43077.638129976855</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="39.75" customHeight="1">
@@ -1173,7 +1212,7 @@
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="13" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G2" s="13"/>
     </row>
@@ -1205,20 +1244,20 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G4" s="6">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1226,215 +1265,223 @@
         <v>18</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G5" s="6">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="G6" s="6">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>20</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="F7" s="6" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="G7" s="6">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="6" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="G9" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
       <c r="F10" s="6" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="G10" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F11" s="6"/>
       <c r="G11" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="G12" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="G13" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="G14" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="6" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>47</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="6"/>
+      <c r="E15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G15" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="6" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7"/>
@@ -1445,67 +1492,67 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="F17" s="6"/>
       <c r="G17" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="6"/>
+        <v>45</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="E18" s="7"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="6"/>
+        <v>67</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="E19" s="7"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="6" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
       <c r="F20" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G20" s="6">
         <v>2</v>
@@ -1513,15 +1560,15 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="6" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6">
@@ -1530,35 +1577,69 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="6" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="E22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="6"/>
       <c r="G22" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="6" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="E23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="6"/>
       <c r="G23" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Statistikk for 9. Desember
</commit_message>
<xml_diff>
--- a/X-Helg 2017 Statistikk.xlsx
+++ b/X-Helg 2017 Statistikk.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\xhelg-stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\xhelg-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18180" windowHeight="5925"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18180" windowHeight="5925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$26</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$29</definedName>
+    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$30</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="statistikk" type="6" refreshedVersion="5" background="1" refreshOnLoad="1" saveData="1">
-    <textPr sourceFile="C:\Code\xhelg-stats\X-Helg_2017_statistikk.csv" decimal="," thousands=" " tab="0" comma="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="statistikk" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
+    <textPr sourceFile="E:\Code\xhelg-stats\X-Helg_2017_statistikk.csv" decimal="," thousands=" " tab="0" comma="1">
       <textFields count="6">
         <textField type="text"/>
         <textField type="text"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>Nick</t>
   </si>
@@ -111,9 +111,6 @@
     <t>TeamLadybug&lt;3&lt;3</t>
   </si>
   <si>
-    <t>[#1]  (1)</t>
-  </si>
-  <si>
     <t>[#2]  (1)</t>
   </si>
   <si>
@@ -195,18 +192,9 @@
     <t>Team Takoma</t>
   </si>
   <si>
-    <t>[#5]  (2)</t>
-  </si>
-  <si>
     <t>[#4]  (1)</t>
   </si>
   <si>
-    <t>[#2] [#5] [#8]  (6)</t>
-  </si>
-  <si>
-    <t>[#1] [#3] [#4] [#6]  (4)</t>
-  </si>
-  <si>
     <t>[#5] [#4] [#6]  (3)</t>
   </si>
   <si>
@@ -222,18 +210,12 @@
     <t>[#6]  (3)</t>
   </si>
   <si>
-    <t>[#1] [#2] [#6] [#3]  (4)</t>
-  </si>
-  <si>
     <t>[#1] [#3] [#6]  (3)</t>
   </si>
   <si>
     <t>[#8]  (2)</t>
   </si>
   <si>
-    <t>[#2] [#6] [#3]  (3)</t>
-  </si>
-  <si>
     <t>anila65</t>
   </si>
   <si>
@@ -258,23 +240,44 @@
     <t>goo.gl/EN6aLd</t>
   </si>
   <si>
-    <t>[#2]* [#8] [#5] [#4]  (11)</t>
-  </si>
-  <si>
     <t>Breimorampen</t>
   </si>
   <si>
     <t>[#7]  (3)</t>
   </si>
   <si>
-    <t>50 besøk fra 23 team!</t>
+    <t>[#2]* [#8] [#5] [#4] [#7]  (14)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#5] [#7] [#8]  (10)</t>
+  </si>
+  <si>
+    <t>[#3] [#4] [#6]  (3)</t>
+  </si>
+  <si>
+    <t>[#2] [#6] [#3] [#5] [#4] [#8]  (6)</t>
+  </si>
+  <si>
+    <t>[#5] [#8]  (4)</t>
+  </si>
+  <si>
+    <t>Team Leteglede</t>
+  </si>
+  <si>
+    <t>[#7]  (2)</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>59 besøk fra 23 team!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -845,24 +848,24 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20 % - uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - uthevingsfarge 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - uthevingsfarge 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - uthevingsfarge 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % – uthevingsfarge 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % – uthevingsfarge 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % – uthevingsfarge 6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Beregning" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Dårlig" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Forklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -903,7 +906,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="statistikk" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="statistikk" refreshOnLoad="1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1202,45 +1205,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="16">
         <f ca="1">NOW()</f>
-        <v>43077.666753356483</v>
+        <v>43078.462146180558</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="39.75" customHeight="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
@@ -1250,11 +1253,11 @@
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="15.75">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1277,28 +1280,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="G4" s="5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -1310,16 +1313,16 @@
         <v>16</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G5" s="5">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
@@ -1331,189 +1334,191 @@
         <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G6" s="5">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="E7" s="6" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G7" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="E8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="5"/>
       <c r="G8" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="5" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="5">
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="5" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>63</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F12" s="5"/>
       <c r="G12" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="F13" s="5" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G13" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>5</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="5" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="G14" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="E15" s="6"/>
       <c r="F15" s="5" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="G15" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>14</v>
@@ -1528,15 +1533,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
@@ -1545,15 +1550,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
@@ -1562,15 +1567,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
@@ -1579,15 +1584,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
@@ -1596,105 +1601,122 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
       <c r="F21" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="E25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="5"/>
       <c r="G25" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
       <c r="F26" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1706,7 +1728,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F1" r:id="rId1"/>
+    <hyperlink ref="F1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="85" orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>

</xml_diff>

<commit_message>
Statistikk for 10. Desember
</commit_message>
<xml_diff>
--- a/X-Helg 2017 Statistikk.xlsx
+++ b/X-Helg 2017 Statistikk.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$27</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$30</definedName>
+    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$32</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="85">
   <si>
     <t>Nick</t>
   </si>
@@ -90,9 +90,6 @@
     <t>johs1988</t>
   </si>
   <si>
-    <t>[#3]* [#2]*  (4)</t>
-  </si>
-  <si>
     <t>siljejandersen</t>
   </si>
   <si>
@@ -195,12 +192,6 @@
     <t>[#4]  (1)</t>
   </si>
   <si>
-    <t>[#5] [#4] [#6]  (3)</t>
-  </si>
-  <si>
-    <t>[#2] [#3] [#5] [#4] [#6]  (5)</t>
-  </si>
-  <si>
     <t>[#1] [#2] [#6]  (6)</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>anila65</t>
   </si>
   <si>
-    <t>[#6] [#1] [#2] [#3]  (4)</t>
-  </si>
-  <si>
     <t>TeamAlmli</t>
   </si>
   <si>
@@ -246,18 +234,12 @@
     <t>[#7]  (3)</t>
   </si>
   <si>
-    <t>[#2]* [#8] [#5] [#4] [#7]  (14)</t>
-  </si>
-  <si>
     <t>[#1] [#2] [#5] [#7] [#8]  (10)</t>
   </si>
   <si>
     <t>[#3] [#4] [#6]  (3)</t>
   </si>
   <si>
-    <t>[#2] [#6] [#3] [#5] [#4] [#8]  (6)</t>
-  </si>
-  <si>
     <t>[#5] [#8]  (4)</t>
   </si>
   <si>
@@ -270,7 +252,49 @@
     <t>11</t>
   </si>
   <si>
-    <t>59 besøk fra 23 team!</t>
+    <t>[#2]* [#4] [#5] [#7] [#8]  (14)</t>
+  </si>
+  <si>
+    <t>[#2]* [#3]*  (4)</t>
+  </si>
+  <si>
+    <t>[#4] [#5] [#6]  (3)</t>
+  </si>
+  <si>
+    <t>[#6]*  (2)</t>
+  </si>
+  <si>
+    <t>[#1] [#6]  (4)</t>
+  </si>
+  <si>
+    <t>[#2] [#3] [#4] [#5] [#8]  (5)</t>
+  </si>
+  <si>
+    <t>[#2] [#3] [#4] [#5] [#6]  (5)</t>
+  </si>
+  <si>
+    <t>[#2] [#3] [#4] [#5] [#6] [#8]  (6)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#6] [#3]  (4)</t>
+  </si>
+  <si>
+    <t>Brustadteam</t>
+  </si>
+  <si>
+    <t>[#9]  (3)</t>
+  </si>
+  <si>
+    <t>Linolse</t>
+  </si>
+  <si>
+    <t>[#10]  (3)</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>59 besøk fra 26 team!</t>
   </si>
 </sst>
 </file>
@@ -1209,10 +1233,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,14 +1257,14 @@
       <c r="B1" s="10"/>
       <c r="C1" s="16">
         <f ca="1">NOW()</f>
-        <v>43078.462146180558</v>
+        <v>43079.502678819445</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1253,7 +1277,7 @@
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="15" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G2" s="15"/>
     </row>
@@ -1285,17 +1309,17 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G4" s="5">
         <v>27</v>
@@ -1303,20 +1327,20 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="G5" s="5">
         <v>13</v>
@@ -1324,20 +1348,20 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="G6" s="5">
         <v>11</v>
@@ -1345,20 +1369,20 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G7" s="5">
         <v>11</v>
@@ -1366,58 +1390,60 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="G8" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>71</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F9" s="5"/>
       <c r="G9" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G10" s="5">
         <v>7</v>
@@ -1425,18 +1451,18 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G11" s="5">
         <v>6</v>
@@ -1447,14 +1473,14 @@
         <v>46</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5">
@@ -1466,15 +1492,15 @@
         <v>46</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G13" s="5">
         <v>5</v>
@@ -1482,16 +1508,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="5" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="G14" s="5">
         <v>4</v>
@@ -1499,7 +1525,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>3</v>
@@ -1510,7 +1536,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="5">
         <v>4</v>
@@ -1518,7 +1544,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>14</v>
@@ -1535,13 +1561,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
@@ -1552,13 +1578,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
@@ -1569,13 +1595,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
@@ -1586,13 +1612,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="C20" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
@@ -1603,66 +1629,66 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="F21" s="5"/>
       <c r="G21" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="E22" s="6"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="G23" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5">
@@ -1671,15 +1697,15 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5">
@@ -1688,35 +1714,69 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="E26" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="5"/>
       <c r="G26" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="E27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="5"/>
       <c r="G27" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Statistikk for 12. Desember
</commit_message>
<xml_diff>
--- a/X-Helg 2017 Statistikk.xlsx
+++ b/X-Helg 2017 Statistikk.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$29</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$32</definedName>
+    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$38</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
   <si>
     <t>Nick</t>
   </si>
@@ -258,9 +258,6 @@
     <t>[#10]  (3)</t>
   </si>
   <si>
-    <t>59 besøk fra 26 team!</t>
-  </si>
-  <si>
     <t>[#1] [#2] [#3] [#5] [#6] [#7] [#8]  (14)</t>
   </si>
   <si>
@@ -270,19 +267,70 @@
     <t>[#1] [#2] [#6] [#8]  (8)</t>
   </si>
   <si>
-    <t>[#3] [#4] [#5]  (3)</t>
-  </si>
-  <si>
     <t>[#3] [#6]  (4)</t>
   </si>
   <si>
-    <t>[#1]  (1)</t>
-  </si>
-  <si>
     <t>[#6]  (2)</t>
   </si>
   <si>
-    <t>[#1] [#2] [#3]  (3)</t>
+    <t>[#4] [#10]  (2)</t>
+  </si>
+  <si>
+    <t>[#3] [#4] [#5] [#10]  (4)</t>
+  </si>
+  <si>
+    <t>[#1] [#10]  (2)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#3] [#10]  (4)</t>
+  </si>
+  <si>
+    <t>[#12]  (3)</t>
+  </si>
+  <si>
+    <t>Team_Alpha300</t>
+  </si>
+  <si>
+    <t>[#11]  (3)</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Askeladdene</t>
+  </si>
+  <si>
+    <t>[#11]  (2)</t>
+  </si>
+  <si>
+    <t>[#2] [#1]  (2)</t>
+  </si>
+  <si>
+    <t>wivian59</t>
+  </si>
+  <si>
+    <t>[#6] [#10]  (2)</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Team Skartun</t>
+  </si>
+  <si>
+    <t>[#9]  (1)</t>
+  </si>
+  <si>
+    <t>hjelpetrollan</t>
+  </si>
+  <si>
+    <t>smøløen</t>
+  </si>
+  <si>
+    <t>[#11]  (1)</t>
+  </si>
+  <si>
+    <t>72 besøk fra 32 team!</t>
   </si>
 </sst>
 </file>
@@ -1221,10 +1269,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,7 +1282,7 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1245,7 +1293,7 @@
       <c r="B1" s="10"/>
       <c r="C1" s="16">
         <f ca="1">NOW()</f>
-        <v>43079.527055902778</v>
+        <v>43081.785657175926</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="11" t="s">
@@ -1265,7 +1313,7 @@
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="15" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="G2" s="15"/>
     </row>
@@ -1304,7 +1352,7 @@
         <v>65</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>48</v>
@@ -1325,13 +1373,13 @@
         <v>66</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="G5" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1346,13 +1394,13 @@
         <v>66</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="G6" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1367,13 +1415,13 @@
         <v>67</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G7" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1388,13 +1436,13 @@
         <v>67</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G8" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1402,46 +1450,46 @@
         <v>23</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>5</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="G9" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>78</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F10" s="5"/>
       <c r="G10" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>30</v>
@@ -1460,106 +1508,108 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="G12" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F13" s="5"/>
       <c r="G13" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>80</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F14" s="5"/>
       <c r="G14" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="5">
         <v>5</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="5">
-        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="G16" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
@@ -1570,13 +1620,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
@@ -1587,13 +1637,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
@@ -1604,13 +1654,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
@@ -1621,13 +1671,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
@@ -1638,13 +1688,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
@@ -1655,49 +1705,49 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
-      <c r="F23" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="F23" s="5"/>
       <c r="G23" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="D24" s="5"/>
-      <c r="E24" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="E24" s="6"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="6" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5">
@@ -1706,27 +1756,27 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="G26" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1740,24 +1790,24 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="E28" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="5"/>
       <c r="G28" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>46</v>
@@ -1766,9 +1816,111 @@
       <c r="D29" s="5"/>
       <c r="E29" s="6"/>
       <c r="F29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G35" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Statistikk for 14. Desember
</commit_message>
<xml_diff>
--- a/X-Helg 2017 Statistikk.xlsx
+++ b/X-Helg 2017 Statistikk.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$38</definedName>
+    <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$41</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="109">
   <si>
     <t>Nick</t>
   </si>
@@ -243,9 +243,6 @@
     <t>[#2]* [#3]*  (4)</t>
   </si>
   <si>
-    <t>[#6]*  (2)</t>
-  </si>
-  <si>
     <t>Brustadteam</t>
   </si>
   <si>
@@ -258,12 +255,6 @@
     <t>[#10]  (3)</t>
   </si>
   <si>
-    <t>[#1] [#2] [#3] [#5] [#6] [#7] [#8]  (14)</t>
-  </si>
-  <si>
-    <t>[#3] [#6]  (4)</t>
-  </si>
-  <si>
     <t>[#1] [#10]  (2)</t>
   </si>
   <si>
@@ -309,22 +300,73 @@
     <t>[#11]  (1)</t>
   </si>
   <si>
-    <t>72 besøk fra 32 team!</t>
-  </si>
-  <si>
-    <t>[#1] [#2] [#3] [#5] [#6] [#10]  (12)</t>
-  </si>
-  <si>
-    <t>[#1] [#2] [#6] [#8] [#10]  (10)</t>
-  </si>
-  <si>
     <t>[#3] [#4] [#5]  (3)</t>
   </si>
   <si>
-    <t>[#6] [#10]  (4)</t>
-  </si>
-  <si>
     <t>[#1] [#2] [#3]  (3)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#3] [#5] [#6] [#7] [#8] [#13]  (16)</t>
+  </si>
+  <si>
+    <t>[#4] [#12] [#10]  (3)</t>
+  </si>
+  <si>
+    <t>[#12]* [#6]*  (4)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#6] [#8] [#10] [#12] [#13]  (14)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#3] [#5] [#6] [#10] [#13]  (14)</t>
+  </si>
+  <si>
+    <t>[#4] [#14]  (2)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#6] [#8] [#10] [#13]  (12)</t>
+  </si>
+  <si>
+    <t>[#3] [#4] [#5] [#12]  (4)</t>
+  </si>
+  <si>
+    <t>[#6] [#10] [#12] [#13] [#14]  (10)</t>
+  </si>
+  <si>
+    <t>[#3] [#6] [#13]  (6)</t>
+  </si>
+  <si>
+    <t>[#14]  (3)</t>
+  </si>
+  <si>
+    <t>[#2] [#13]  (4)</t>
+  </si>
+  <si>
+    <t>[#13]  (2)</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>IFYELife</t>
+  </si>
+  <si>
+    <t>brennes</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Hegeka&amp;co</t>
+  </si>
+  <si>
+    <t>[#12]  (1)</t>
+  </si>
+  <si>
+    <t>93 besøk fra 35 team!</t>
   </si>
 </sst>
 </file>
@@ -1263,10 +1305,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1318,7 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1287,7 +1329,7 @@
       <c r="B1" s="10"/>
       <c r="C1" s="16">
         <f ca="1">NOW()</f>
-        <v>43081.795854282405</v>
+        <v>43083.960950925924</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="11" t="s">
@@ -1307,7 +1349,7 @@
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="15" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="G2" s="15"/>
     </row>
@@ -1334,7 +1376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1346,55 +1388,55 @@
         <v>65</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="G4" s="5">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="G5" s="5">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
         <v>66</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="G6" s="5">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1402,93 +1444,93 @@
         <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G7" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="G8" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="G9" s="5">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>5</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="G10" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6" t="s">
         <v>49</v>
@@ -1497,60 +1539,62 @@
         <v>50</v>
       </c>
       <c r="G11" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E12" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>94</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F12" s="5"/>
       <c r="G12" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5">
@@ -1559,102 +1603,108 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D15" s="5"/>
       <c r="E15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5">
         <v>5</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="5">
-        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="G18" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="G19" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
@@ -1665,13 +1715,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
@@ -1682,13 +1732,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
@@ -1699,13 +1749,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
@@ -1716,13 +1766,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
@@ -1733,15 +1783,15 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5">
@@ -1750,49 +1800,49 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="E26" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="5"/>
       <c r="G26" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="G27" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="6" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5">
@@ -1801,32 +1851,32 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="5" t="s">
-        <v>81</v>
-      </c>
+      <c r="E29" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="5"/>
       <c r="G29" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="6" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5">
@@ -1835,16 +1885,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="6"/>
       <c r="F31" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G31" s="5">
         <v>2</v>
@@ -1852,50 +1902,50 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="E32" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="5"/>
       <c r="G32" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
       <c r="F33" s="5" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="G33" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
       <c r="F34" s="5" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="G34" s="5">
         <v>1</v>
@@ -1903,18 +1953,69 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
       <c r="F35" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G35" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Statistikk for 22. Desember
</commit_message>
<xml_diff>
--- a/X-Helg 2017 Statistikk.xlsx
+++ b/X-Helg 2017 Statistikk.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\xhelg-stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\xhelg-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18180" windowHeight="5925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18180" windowHeight="5925"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <definedName name="statistikk" localSheetId="0">'Ark1'!$A$3:$G$46</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Ark1'!$A$1:$G$49</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="statistikk" type="6" refreshedVersion="6" background="1" refreshOnLoad="1" saveData="1">
-    <textPr sourceFile="E:\Code\xhelg-stats\X-Helg_2017_statistikk.csv" decimal="," thousands=" " tab="0" comma="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="statistikk" type="6" refreshedVersion="5" background="1" refreshOnLoad="1" saveData="1">
+    <textPr sourceFile="C:\Code\xhelg-stats\X-Helg_2017_statistikk.csv" decimal="," thousands=" " tab="0" comma="1">
       <textFields count="6">
         <textField type="text"/>
         <textField type="text"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="138">
   <si>
     <t>Nick</t>
   </si>
@@ -213,18 +213,12 @@
     <t>[#7]  (3)</t>
   </si>
   <si>
-    <t>[#5] [#8]  (4)</t>
-  </si>
-  <si>
     <t>Team Leteglede</t>
   </si>
   <si>
     <t>[#7]  (2)</t>
   </si>
   <si>
-    <t>[#2]* [#3]*  (4)</t>
-  </si>
-  <si>
     <t>Brustadteam</t>
   </si>
   <si>
@@ -279,21 +273,9 @@
     <t>[#11]  (1)</t>
   </si>
   <si>
-    <t>[#3] [#4] [#5]  (3)</t>
-  </si>
-  <si>
-    <t>[#4] [#12] [#10]  (3)</t>
-  </si>
-  <si>
     <t>[#1] [#2] [#3] [#5] [#6] [#10] [#13]  (14)</t>
   </si>
   <si>
-    <t>[#3] [#4] [#5] [#12]  (4)</t>
-  </si>
-  <si>
-    <t>[#6] [#10] [#12] [#13] [#14]  (10)</t>
-  </si>
-  <si>
     <t>[#3] [#6] [#13]  (6)</t>
   </si>
   <si>
@@ -342,15 +324,9 @@
     <t>[#14]  (1)</t>
   </si>
   <si>
-    <t>[#2]* [#14] [#4] [#5] [#7] [#8]  (17)</t>
-  </si>
-  <si>
     <t>[#16]  (3)</t>
   </si>
   <si>
-    <t>[#3] [#12] [#4] [#5] [#8]  (5)</t>
-  </si>
-  <si>
     <t>[#2] [#13] [#16]  (6)</t>
   </si>
   <si>
@@ -372,9 +348,6 @@
     <t>[#18]  (3)</t>
   </si>
   <si>
-    <t>[#1] [#2] [#3] [#5] [#6] [#7] [#8] [#13] [#14] [#16] [#17]  (22)</t>
-  </si>
-  <si>
     <t>[#4] [#14] [#16] [#18]  (4)</t>
   </si>
   <si>
@@ -384,24 +357,12 @@
     <t>[#4] [#14] [#18]  (3)</t>
   </si>
   <si>
-    <t>[#1] [#2] [#3] [#16] [#18]  (5)</t>
-  </si>
-  <si>
-    <t>[#1] [#10] [#16] [#12] [#14] [#18]  (6)</t>
-  </si>
-  <si>
     <t>[#1] [#13]  (4)</t>
   </si>
   <si>
-    <t>[#14] [#16]  (2)</t>
-  </si>
-  <si>
     <t>[#7]  (1)</t>
   </si>
   <si>
-    <t>[#4] [#18]  (2)</t>
-  </si>
-  <si>
     <t>joooliii</t>
   </si>
   <si>
@@ -411,15 +372,6 @@
     <t>skogmal</t>
   </si>
   <si>
-    <t>[#12]* [#18]* [#6]*  (6)</t>
-  </si>
-  <si>
-    <t>[#1] [#2] [#6] [#8] [#10] [#12] [#13] [#14] [#16] [#18]  (20)</t>
-  </si>
-  <si>
-    <t>[#1] [#2] [#6] [#8] [#10] [#13] [#14] [#16] [#18]  (18)</t>
-  </si>
-  <si>
     <t>[#20]  (3)</t>
   </si>
   <si>
@@ -435,14 +387,80 @@
     <t>[#20]  (1)</t>
   </si>
   <si>
-    <t>133 besøk fra 43 team!</t>
+    <t>[#2]* [#14] [#8] [#5] [#4] [#7]  (17)</t>
+  </si>
+  <si>
+    <t>[#6]* [#18]* [#12]*  (6)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#6] [#8] [#10] [#12] [#13] [#14] [#16] [#18] [#21]  (22)</t>
+  </si>
+  <si>
+    <t>[#3] [#5] [#4]  (3)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#6] [#8] [#10] [#13] [#14] [#16] [#18] [#21]  (20)</t>
+  </si>
+  <si>
+    <t>[#3] [#5] [#4] [#12]  (4)</t>
+  </si>
+  <si>
+    <t>[#16] [#22] [#21]  (9)</t>
+  </si>
+  <si>
+    <t>[#6] [#10] [#12] [#13] [#14] [#22]  (12)</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#3] [#16] [#18] [#21]  (6)</t>
+  </si>
+  <si>
+    <t>[#22]  (3)</t>
+  </si>
+  <si>
+    <t>[#3]* [#2]*  (4)</t>
+  </si>
+  <si>
+    <t>[#21]  (3)</t>
+  </si>
+  <si>
+    <t>[#3] [#12] [#8] [#5] [#4]  (5)</t>
+  </si>
+  <si>
+    <t>[#1] [#10] [#16] [#18] [#12] [#14]  (6)</t>
+  </si>
+  <si>
+    <t>[#16] [#18]  (2)</t>
+  </si>
+  <si>
+    <t>[#16] [#14]  (2)</t>
+  </si>
+  <si>
+    <t>[#16] [#14] [#18] [#10]  (4)</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>143 besøk fra 43 team!</t>
+  </si>
+  <si>
+    <t>[#1] [#2] [#3] [#5] [#4] [#6] [#7] [#8] [#12] [#13] [#14] [#16] [#17] [#21] [#22]  (30)</t>
+  </si>
+  <si>
+    <t>[#10]  (1)</t>
+  </si>
+  <si>
+    <t>[#5] [#4] [#8]  (6)</t>
+  </si>
+  <si>
+    <t>[#18]  (1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1013,24 +1031,24 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20 % – uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % – uthevingsfarge 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % – uthevingsfarge 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % – uthevingsfarge 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % – uthevingsfarge 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % – uthevingsfarge 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % – uthevingsfarge 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % – uthevingsfarge 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % – uthevingsfarge 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % – uthevingsfarge 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % – uthevingsfarge 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % – uthevingsfarge 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % – uthevingsfarge 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % – uthevingsfarge 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % – uthevingsfarge 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % – uthevingsfarge 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % – uthevingsfarge 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % – uthevingsfarge 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % - uthevingsfarge 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - uthevingsfarge 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - uthevingsfarge 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - uthevingsfarge 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - uthevingsfarge 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - uthevingsfarge 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - uthevingsfarge 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - uthevingsfarge 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - uthevingsfarge 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - uthevingsfarge 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - uthevingsfarge 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - uthevingsfarge 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - uthevingsfarge 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - uthevingsfarge 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - uthevingsfarge 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - uthevingsfarge 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - uthevingsfarge 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - uthevingsfarge 6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Beregning" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Dårlig" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Forklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1071,7 +1089,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="statistikk" refreshOnLoad="1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="statistikk" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1370,7 +1388,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1380,7 +1398,7 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
@@ -1391,14 +1409,14 @@
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="16">
         <f ca="1">NOW()</f>
-        <v>43089.84983078704</v>
+        <v>43091.81162291667</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="11" t="s">
@@ -1408,7 +1426,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="39.75" customHeight="1">
       <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
@@ -1418,11 +1436,11 @@
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="15" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="15.75">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1445,7 +1463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="75">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1453,22 +1471,22 @@
         <v>24</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="G4" s="5">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="60">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -1477,19 +1495,19 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="G5" s="5">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1498,107 +1516,111 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="G6" s="5">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>60</v>
+        <v>121</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="G7" s="5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>102</v>
       </c>
       <c r="G8" s="5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="D9" s="5" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="G9" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30">
+      <c r="A10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G10" s="5">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G10" s="5">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
@@ -1608,18 +1630,18 @@
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="G11" s="5">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>21</v>
@@ -1631,56 +1653,56 @@
         <v>5</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="G14" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>61</v>
@@ -1690,153 +1712,155 @@
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="G15" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="G16" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="6" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="G17" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>126</v>
+        <v>60</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>80</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="G18" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>80</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="G19" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
-        <v>64</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="6" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="5" t="s">
-        <v>117</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="5"/>
       <c r="G21" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>38</v>
@@ -1853,26 +1877,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>40</v>
@@ -1887,9 +1911,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>49</v>
@@ -1904,9 +1928,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>55</v>
@@ -1921,15 +1945,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
@@ -1938,15 +1962,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="6"/>
@@ -1955,15 +1979,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="6"/>
@@ -1972,15 +1996,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="6"/>
@@ -1989,26 +2013,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>28</v>
@@ -2017,15 +2041,15 @@
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
       <c r="F33" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G33" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>33</v>
@@ -2040,26 +2064,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>44</v>
@@ -2068,32 +2092,32 @@
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
       <c r="F36" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G36" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>36</v>
@@ -2108,77 +2132,77 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G39" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="6"/>
       <c r="F40" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G40" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="6"/>
       <c r="F41" s="5" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="G41" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="6"/>
       <c r="F42" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G42" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>35</v>
@@ -2193,52 +2217,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="6"/>
       <c r="F44" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G44" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="6"/>
       <c r="F45" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G45" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="6"/>
       <c r="F46" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G46" s="5">
         <v>1</v>
@@ -2252,7 +2276,7 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="83" orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>

</xml_diff>